<commit_message>
6/10/2015 More sample code
</commit_message>
<xml_diff>
--- a/public_html/CIT261.xlsx
+++ b/public_html/CIT261.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
   <si>
     <t>Current Overall Score*</t>
   </si>
@@ -77,9 +77,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>passed</t>
-  </si>
-  <si>
     <t>App Design and Creation</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
     <t>Local Storage API, Storing and Retrieving Simple Data, Arrays, Associative Arrays, and Objects</t>
   </si>
   <si>
+    <t>created</t>
+  </si>
+  <si>
     <t>Journal Report</t>
   </si>
   <si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Manipulating CSS Class Properties Using JavaScript</t>
+  </si>
+  <si>
+    <t>not created</t>
   </si>
   <si>
     <t>Using XMLHTTPRequest to Consume a JSON Web Service</t>
@@ -563,8 +566,8 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -587,7 +590,7 @@
       </c>
       <c r="C1" s="3" t="n">
         <f aca="false">I13*J7+I21*J8+H29*J9+H36*J10+H44*J11</f>
-        <v>0</v>
+        <v>0.408722222222222</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -717,15 +720,13 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="13" t="s">
+      <c r="E8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="13"/>
+      <c r="I8" s="19" t="s">
         <v>20</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>21</v>
       </c>
       <c r="J8" s="15" t="n">
         <v>0.29</v>
@@ -739,20 +740,20 @@
     </row>
     <row r="9" customFormat="false" ht="49.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="6"/>
       <c r="G9" s="13"/>
       <c r="I9" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J9" s="15" t="n">
         <v>0.22</v>
@@ -767,19 +768,17 @@
     <row r="10" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
       <c r="B10" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="E10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="13"/>
       <c r="I10" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="15" t="n">
         <v>0.07</v>
@@ -794,7 +793,7 @@
     <row r="11" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
       <c r="B11" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -802,7 +801,9 @@
       <c r="F11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="I11" s="14" t="s">
         <v>28</v>
       </c>
@@ -817,10 +818,10 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="6"/>
       <c r="G12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -834,12 +835,15 @@
       <c r="F13" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="G13" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="H13" s="13" t="s">
         <v>31</v>
       </c>
       <c r="I13" s="21" t="n">
         <f aca="false">((COUNTIF(C8:C16,"&gt;''"))+(COUNTIF(D8:D16,"&gt;''")*M8)+(COUNTIF(E8:E16,"&gt;''")*M9))/9</f>
-        <v>0</v>
+        <v>0.297777777777778</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -853,12 +857,14 @@
       <c r="F14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13"/>
       <c r="B15" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -866,12 +872,14 @@
       <c r="F15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -879,9 +887,11 @@
       <c r="F16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="6"/>
@@ -890,7 +900,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="G18" s="13"/>
@@ -898,7 +908,7 @@
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
       <c r="B19" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>12</v>
@@ -917,39 +927,39 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="6"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="B21" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="6"/>
       <c r="H21" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I21" s="21" t="n">
         <f aca="false">((COUNTIF(C20:C24,"&gt;''"))+(COUNTIF(D20:D24,"&gt;''")*M8)+(COUNTIF(E20:E24,"&gt;''")*M9))/5</f>
-        <v>0</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -957,27 +967,27 @@
       <c r="F22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>20</v>
-      </c>
+      <c r="E23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -985,7 +995,9 @@
       <c r="F24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="13"/>
+      <c r="G24" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="22"/>
@@ -996,13 +1008,13 @@
       <c r="F25" s="5"/>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="13"/>
       <c r="G26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>12</v>
@@ -1020,44 +1032,44 @@
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="6"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="6"/>
       <c r="G29" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H29" s="21" t="str">
+        <v>48</v>
+      </c>
+      <c r="H29" s="21" t="n">
         <f aca="false">((COUNTIF(C28:C32,"&gt;''"))+(COUNTIF(D28:D32,"&gt;''")*M8)+(COUNTIF(E28:E32,"&gt;''")*M9))/5</f>
-        <v>0%</v>
+        <v>0.536</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1070,27 +1082,27 @@
     <row r="31" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="13"/>
       <c r="B31" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="6"/>
       <c r="G31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="13"/>
       <c r="B32" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="E32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="6"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,40 +1126,40 @@
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="26" t="s">
-        <v>19</v>
-      </c>
+      <c r="F36" s="26"/>
       <c r="G36" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H36" s="27" t="str">
+        <v>58</v>
+      </c>
+      <c r="H36" s="27" t="n">
         <f aca="false">((COUNTIF(C36,"&gt;''"))+(COUNTIF(D36,"&gt;''")*M8)+(COUNTIF(E36,"&gt;''")*M9))</f>
-        <v>0%</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,7 +1173,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="6"/>
@@ -1189,7 +1201,7 @@
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -1208,7 +1220,7 @@
     <row r="42" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="13"/>
       <c r="B42" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1221,7 +1233,7 @@
     <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="13"/>
       <c r="B43" s="13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1234,7 +1246,7 @@
     <row r="44" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="13"/>
       <c r="B44" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1243,7 +1255,7 @@
         <v>19</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H44" s="21" t="str">
         <f aca="false">((COUNTIF(C42:C45,"&gt;''"))+(COUNTIF(D42:D45,"&gt;''")*M8)+(COUNTIF(E42:E45,"&gt;''")*M9))/4</f>
@@ -1253,7 +1265,7 @@
     <row r="45" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -1263,6 +1275,9 @@
       </c>
       <c r="G45" s="13"/>
     </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
6/11/2015 Hunter's event code and some java animations
</commit_message>
<xml_diff>
--- a/public_html/CIT261.xlsx
+++ b/public_html/CIT261.xlsx
@@ -98,7 +98,7 @@
     <t>Local Storage API, Storing and Retrieving Simple Data, Arrays, Associative Arrays, and Objects</t>
   </si>
   <si>
-    <t>created</t>
+    <t>passed off</t>
   </si>
   <si>
     <t>Journal Report</t>
@@ -566,8 +566,8 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -968,7 +968,7 @@
         <v>19</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
6/19/2015 Game files for the top down shooter and personal project files
</commit_message>
<xml_diff>
--- a/public_html/CIT261.xlsx
+++ b/public_html/CIT261.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Current Overall Score*</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Local Storage API, Storing and Retrieving Simple Data, Arrays, Associative Arrays, and Objects</t>
   </si>
   <si>
-    <t>passed off</t>
-  </si>
-  <si>
     <t>Journal Report</t>
   </si>
   <si>
@@ -116,10 +113,10 @@
     <t>Manipulating CSS Class Properties Using JavaScript</t>
   </si>
   <si>
+    <t>Using XMLHTTPRequest to Consume a JSON Web Service</t>
+  </si>
+  <si>
     <t>not created</t>
-  </si>
-  <si>
-    <t>Using XMLHTTPRequest to Consume a JSON Web Service</t>
   </si>
   <si>
     <t>Standard JavaScript Events Including those for Mobile Devices ( Ex. onTouchBegin, onLoad, etc.)</t>
@@ -566,8 +563,8 @@
   </sheetPr>
   <dimension ref="A1:M65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -590,7 +587,7 @@
       </c>
       <c r="C1" s="3" t="n">
         <f aca="false">I13*J7+I21*J8+H29*J9+H36*J10+H44*J11</f>
-        <v>0.408722222222222</v>
+        <v>0.545548888888889</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -797,15 +794,13 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="13" t="s">
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="13"/>
+      <c r="I11" s="14" t="s">
         <v>27</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="J11" s="15" t="n">
         <v>0.07</v>
@@ -814,7 +809,7 @@
     <row r="12" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -827,44 +822,39 @@
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
       <c r="B13" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>27</v>
-      </c>
+      <c r="E13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="H13" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" s="21" t="n">
         <f aca="false">((COUNTIF(C8:C16,"&gt;''"))+(COUNTIF(D8:D16,"&gt;''")*M8)+(COUNTIF(E8:E16,"&gt;''")*M9))/9</f>
-        <v>0.297777777777778</v>
+        <v>0.521111111111111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
       <c r="B14" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>33</v>
-      </c>
+      <c r="E14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13"/>
       <c r="B15" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -879,7 +869,7 @@
     <row r="16" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
       <c r="B16" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -908,7 +898,7 @@
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
       <c r="B19" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>12</v>
@@ -927,7 +917,7 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="B20" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -940,7 +930,7 @@
     <row r="21" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="B21" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -949,32 +939,30 @@
       </c>
       <c r="F21" s="6"/>
       <c r="H21" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I21" s="21" t="n">
         <f aca="false">((COUNTIF(C20:C24,"&gt;''"))+(COUNTIF(D20:D24,"&gt;''")*M8)+(COUNTIF(E20:E24,"&gt;''")*M9))/5</f>
-        <v>0.402</v>
+        <v>0.536</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>27</v>
-      </c>
+      <c r="E22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="34.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -987,7 +975,7 @@
     <row r="24" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1014,7 +1002,7 @@
     </row>
     <row r="27" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>12</v>
@@ -1032,44 +1020,44 @@
     </row>
     <row r="28" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>45</v>
-      </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>47</v>
-      </c>
       <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D29" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H29" s="21" t="n">
         <f aca="false">((COUNTIF(C28:C32,"&gt;''"))+(COUNTIF(D28:D32,"&gt;''")*M8)+(COUNTIF(E28:E32,"&gt;''")*M9))/5</f>
-        <v>0.536</v>
+        <v>0.626</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="13"/>
       <c r="B30" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
@@ -1082,7 +1070,7 @@
     <row r="31" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="13"/>
       <c r="B31" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1095,13 +1083,13 @@
     <row r="32" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="13"/>
       <c r="B32" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
-        <v>19</v>
-      </c>
+      <c r="D32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="13"/>
     </row>
@@ -1126,26 +1114,26 @@
     <row r="35" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="D35" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="24" t="s">
+      <c r="E35" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="F35" s="24" t="s">
         <v>55</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>56</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1155,7 +1143,7 @@
       <c r="E36" s="1"/>
       <c r="F36" s="26"/>
       <c r="G36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H36" s="27" t="n">
         <f aca="false">((COUNTIF(C36,"&gt;''"))+(COUNTIF(D36,"&gt;''")*M8)+(COUNTIF(E36,"&gt;''")*M9))</f>
@@ -1173,7 +1161,7 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="6"/>
@@ -1201,7 +1189,7 @@
     </row>
     <row r="41" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>12</v>
@@ -1220,7 +1208,7 @@
     <row r="42" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="13"/>
       <c r="B42" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1233,7 +1221,7 @@
     <row r="43" customFormat="false" ht="46.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="13"/>
       <c r="B43" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1246,7 +1234,7 @@
     <row r="44" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="13"/>
       <c r="B44" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -1255,7 +1243,7 @@
         <v>19</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H44" s="21" t="str">
         <f aca="false">((COUNTIF(C42:C45,"&gt;''"))+(COUNTIF(D42:D45,"&gt;''")*M8)+(COUNTIF(E42:E45,"&gt;''")*M9))/4</f>
@@ -1265,7 +1253,7 @@
     <row r="45" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="13"/>
       <c r="B45" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>

</xml_diff>